<commit_message>
started on grading app
</commit_message>
<xml_diff>
--- a/inst/templates/studentlist_template.xlsx
+++ b/inst/templates/studentlist_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\andreashandel\quizgrader\inst\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB81A3CB-501F-40FF-B4A6-A572057FAF76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48C8548-EB4A-442D-A925-FE7655C1E299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="1395" windowWidth="43395" windowHeight="20565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="course_list_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Password</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>StudentID</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>canbeanything</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -874,9 +886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -928,6 +942,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{7470BC4E-7ED7-472F-A3AF-DD0C79DA9086}"/>

</xml_diff>

<commit_message>
trying to fix it
</commit_message>
<xml_diff>
--- a/inst/templates/studentlist_template.xlsx
+++ b/inst/templates/studentlist_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\andreashandel\quizgrader\inst\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Github\andreashandel\quizgrader\inst\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F604A69-016E-4709-9187-80963E341621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0167A3BE-3F56-49D9-9F63-27250D4C3EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="420" windowWidth="44640" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="course_list_template" sheetId="1" r:id="rId1"/>
@@ -20,32 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Handel</t>
-  </si>
-  <si>
-    <t>Andreas</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>a@b.com</t>
-  </si>
-  <si>
     <t>hello@world.edu</t>
   </si>
   <si>
@@ -58,12 +37,6 @@
     <t>StudentID</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>canbeanything</t>
   </si>
   <si>
@@ -77,13 +50,16 @@
   </si>
   <si>
     <t>Untimed</t>
+  </si>
+  <si>
+    <t>john-smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,14 +190,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -524,7 +492,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -567,14 +535,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -608,7 +576,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -895,118 +862,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="b">
+      <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
+      <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7470BC4E-7ED7-472F-A3AF-DD0C79DA9086}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{455443E9-87CD-4976-B183-AA6413CDE82E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>